<commit_message>
Add ADV-16 code replacement integration test Sample
Ticket: mps#84
</commit_message>
<xml_diff>
--- a/testData/testData_NRL_AR.xlsx
+++ b/testData/testData_NRL_AR.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="219">
   <si>
     <r>
       <rPr>
@@ -634,6 +634,12 @@
     <t xml:space="preserve">Escherichia coli</t>
   </si>
   <si>
+    <t xml:space="preserve">14.09.2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.09.2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">10178</t>
   </si>
   <si>
@@ -664,7 +670,7 @@
     <t xml:space="preserve">Lebensmitteleinzelhandel</t>
   </si>
   <si>
-    <t xml:space="preserve">72,12,16,95,95</t>
+    <t xml:space="preserve">72, 95,95</t>
   </si>
   <si>
     <t xml:space="preserve">Hinweise zum Einsendeformular des BfR:</t>
@@ -3655,9 +3661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>784080</xdr:colOff>
+      <xdr:colOff>783720</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:rowOff>51120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3671,7 +3677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12320280" y="57240"/>
-          <a:ext cx="1757880" cy="622800"/>
+          <a:ext cx="1757520" cy="622440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3693,7 +3699,7 @@
   </sheetPr>
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L36" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="S42" activeCellId="0" sqref="S42"/>
     </sheetView>
   </sheetViews>
@@ -3703,7 +3709,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.99"/>
@@ -3711,7 +3717,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="10.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="10.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="10.58"/>
@@ -3720,7 +3726,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="4" width="5.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="4" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="4" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="4" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="4" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="4" width="8.71"/>
@@ -5238,48 +5244,48 @@
         <v>73</v>
       </c>
       <c r="D42" s="71"/>
-      <c r="E42" s="72" t="n">
-        <v>42992</v>
-      </c>
-      <c r="F42" s="73" t="n">
-        <v>42993</v>
+      <c r="E42" s="72" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="73" t="s">
+        <v>75</v>
       </c>
       <c r="G42" s="74" t="n">
         <v>11000000</v>
       </c>
       <c r="H42" s="75" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="I42" s="76" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J42" s="77" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="K42" s="78" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="L42" s="69" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M42" s="79" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="N42" s="77" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O42" s="69" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="P42" s="70" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q42" s="71" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R42" s="80"/>
       <c r="S42" s="81" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="U42" s="83"/>
     </row>
@@ -5368,7 +5374,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="84" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="84" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="84" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="84" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="84" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="84" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="84" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="84" width="6.71"/>
@@ -5384,7 +5390,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="85" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -5430,7 +5436,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="87" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B3" s="86"/>
       <c r="C3" s="86"/>
@@ -5454,15 +5460,15 @@
     </row>
     <row r="4" customFormat="false" ht="27.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="88" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B4" s="89" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C4" s="89"/>
       <c r="D4" s="89"/>
       <c r="E4" s="89" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F4" s="89"/>
       <c r="G4" s="89"/>
@@ -5476,25 +5482,25 @@
       <c r="O4" s="89"/>
       <c r="P4" s="89"/>
       <c r="Q4" s="90" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="R4" s="90"/>
       <c r="S4" s="91" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="T4" s="91"/>
     </row>
     <row r="5" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="92" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B5" s="93" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C5" s="93"/>
       <c r="D5" s="93"/>
       <c r="E5" s="94" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F5" s="94"/>
       <c r="G5" s="94"/>
@@ -5508,25 +5514,25 @@
       <c r="O5" s="94"/>
       <c r="P5" s="94"/>
       <c r="Q5" s="95" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="R5" s="95"/>
       <c r="S5" s="96" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T5" s="96"/>
     </row>
     <row r="6" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="97" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C6" s="98"/>
       <c r="D6" s="98"/>
       <c r="E6" s="99" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F6" s="99"/>
       <c r="G6" s="99"/>
@@ -5542,21 +5548,21 @@
       <c r="Q6" s="100"/>
       <c r="R6" s="100"/>
       <c r="S6" s="101" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T6" s="101"/>
     </row>
     <row r="7" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="97" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C7" s="98"/>
       <c r="D7" s="98"/>
       <c r="E7" s="99" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F7" s="99"/>
       <c r="G7" s="99"/>
@@ -5570,25 +5576,25 @@
       <c r="O7" s="99"/>
       <c r="P7" s="99"/>
       <c r="Q7" s="100" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="R7" s="100"/>
       <c r="S7" s="102" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="T7" s="102"/>
     </row>
     <row r="8" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="97" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C8" s="98"/>
       <c r="D8" s="98"/>
       <c r="E8" s="99" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F8" s="99"/>
       <c r="G8" s="99"/>
@@ -5608,15 +5614,15 @@
     </row>
     <row r="9" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="97" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B9" s="98" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C9" s="98"/>
       <c r="D9" s="98"/>
       <c r="E9" s="99" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F9" s="99"/>
       <c r="G9" s="99"/>
@@ -5630,17 +5636,17 @@
       <c r="O9" s="99"/>
       <c r="P9" s="99"/>
       <c r="Q9" s="100" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="R9" s="100"/>
       <c r="S9" s="102" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T9" s="102"/>
     </row>
     <row r="10" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="97" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B10" s="98" t="s">
         <v>57</v>
@@ -5648,7 +5654,7 @@
       <c r="C10" s="98"/>
       <c r="D10" s="98"/>
       <c r="E10" s="99" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F10" s="99"/>
       <c r="G10" s="99"/>
@@ -5664,21 +5670,21 @@
       <c r="Q10" s="100"/>
       <c r="R10" s="100"/>
       <c r="S10" s="102" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T10" s="102"/>
     </row>
     <row r="11" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="97" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C11" s="98"/>
       <c r="D11" s="98"/>
       <c r="E11" s="99" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F11" s="99"/>
       <c r="G11" s="99"/>
@@ -5694,21 +5700,21 @@
       <c r="Q11" s="100"/>
       <c r="R11" s="100"/>
       <c r="S11" s="102" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="T11" s="102"/>
     </row>
     <row r="12" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="97" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B12" s="98" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C12" s="98"/>
       <c r="D12" s="98"/>
       <c r="E12" s="99" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F12" s="99"/>
       <c r="G12" s="99"/>
@@ -5728,15 +5734,15 @@
     </row>
     <row r="13" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="97" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B13" s="98" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C13" s="98"/>
       <c r="D13" s="98"/>
       <c r="E13" s="99" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F13" s="99"/>
       <c r="G13" s="99"/>
@@ -5756,15 +5762,15 @@
     </row>
     <row r="14" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="97" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B14" s="103" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C14" s="103"/>
       <c r="D14" s="103"/>
       <c r="E14" s="99" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F14" s="99"/>
       <c r="G14" s="99"/>
@@ -5778,25 +5784,25 @@
       <c r="O14" s="99"/>
       <c r="P14" s="99"/>
       <c r="Q14" s="100" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="R14" s="100"/>
       <c r="S14" s="102" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="T14" s="102"/>
     </row>
     <row r="15" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="97" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B15" s="98" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C15" s="98"/>
       <c r="D15" s="98"/>
       <c r="E15" s="99" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F15" s="99"/>
       <c r="G15" s="99"/>
@@ -5816,15 +5822,15 @@
     </row>
     <row r="16" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="97" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C16" s="98"/>
       <c r="D16" s="98"/>
       <c r="E16" s="99" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F16" s="99"/>
       <c r="G16" s="99"/>
@@ -5844,15 +5850,15 @@
     </row>
     <row r="17" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="97" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B17" s="98" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C17" s="98"/>
       <c r="D17" s="98"/>
       <c r="E17" s="99" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F17" s="99"/>
       <c r="G17" s="99"/>
@@ -5868,21 +5874,21 @@
       <c r="Q17" s="100"/>
       <c r="R17" s="100"/>
       <c r="S17" s="102" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T17" s="102"/>
     </row>
     <row r="18" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="97" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B18" s="98" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C18" s="98"/>
       <c r="D18" s="98"/>
       <c r="E18" s="99" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F18" s="99"/>
       <c r="G18" s="99"/>
@@ -5898,21 +5904,21 @@
       <c r="Q18" s="100"/>
       <c r="R18" s="100"/>
       <c r="S18" s="102" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="T18" s="102"/>
     </row>
     <row r="19" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="97" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B19" s="104" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C19" s="104"/>
       <c r="D19" s="104"/>
       <c r="E19" s="99" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F19" s="99"/>
       <c r="G19" s="99"/>
@@ -5932,15 +5938,15 @@
     </row>
     <row r="20" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="97" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B20" s="98" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C20" s="98"/>
       <c r="D20" s="98"/>
       <c r="E20" s="99" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F20" s="99"/>
       <c r="G20" s="99"/>
@@ -5956,21 +5962,21 @@
       <c r="Q20" s="100"/>
       <c r="R20" s="100"/>
       <c r="S20" s="102" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="T20" s="102"/>
     </row>
     <row r="21" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="97" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B21" s="98" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
       <c r="E21" s="99" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F21" s="99"/>
       <c r="G21" s="99"/>
@@ -5990,15 +5996,15 @@
     </row>
     <row r="22" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="105" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B22" s="106" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C22" s="106"/>
       <c r="D22" s="106"/>
       <c r="E22" s="99" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F22" s="99"/>
       <c r="G22" s="99"/>
@@ -6014,21 +6020,21 @@
       <c r="Q22" s="100"/>
       <c r="R22" s="100"/>
       <c r="S22" s="102" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T22" s="102"/>
     </row>
     <row r="23" customFormat="false" ht="51" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="107" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B23" s="108" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="108"/>
       <c r="E23" s="109" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F23" s="109"/>
       <c r="G23" s="109"/>
@@ -6070,7 +6076,7 @@
     </row>
     <row r="25" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="114" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B25" s="112"/>
       <c r="C25" s="112"/>
@@ -6094,7 +6100,7 @@
     </row>
     <row r="26" s="113" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="115" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B26" s="115"/>
       <c r="C26" s="115"/>
@@ -6140,7 +6146,7 @@
     </row>
     <row r="28" s="113" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="114" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B28" s="112"/>
       <c r="C28" s="112"/>
@@ -6164,7 +6170,7 @@
     </row>
     <row r="29" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="116" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B29" s="117" t="s">
         <v>52</v>
@@ -6173,10 +6179,10 @@
         <v>53</v>
       </c>
       <c r="D29" s="117" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E29" s="119" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F29" s="120" t="s">
         <v>56</v>
@@ -6185,66 +6191,66 @@
         <v>57</v>
       </c>
       <c r="H29" s="117" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I29" s="121" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J29" s="119" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="K29" s="120" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="L29" s="121" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="M29" s="118" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="N29" s="122" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="O29" s="120" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="P29" s="118" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q29" s="117" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="R29" s="119" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="S29" s="123" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="T29" s="124" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="125" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B30" s="126" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C30" s="127" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D30" s="126" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E30" s="76" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F30" s="128" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G30" s="129" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H30" s="130" t="n">
         <v>11000000</v>
@@ -6252,14 +6258,14 @@
       <c r="I30" s="78"/>
       <c r="J30" s="69"/>
       <c r="K30" s="126" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L30" s="131" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="M30" s="132"/>
       <c r="N30" s="133" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="O30" s="130" t="n">
         <v>81</v>
@@ -6270,68 +6276,68 @@
       </c>
       <c r="R30" s="76"/>
       <c r="S30" s="134" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="T30" s="81"/>
     </row>
     <row r="31" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="135" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B31" s="136" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C31" s="137" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D31" s="138"/>
       <c r="E31" s="139" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F31" s="140" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G31" s="141" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H31" s="142"/>
       <c r="I31" s="143" t="n">
         <v>10787</v>
       </c>
       <c r="J31" s="137" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K31" s="138"/>
       <c r="L31" s="144"/>
       <c r="M31" s="137" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N31" s="145"/>
       <c r="O31" s="146"/>
       <c r="P31" s="137" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="Q31" s="138"/>
       <c r="R31" s="139" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="S31" s="147" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="T31" s="148"/>
     </row>
     <row r="32" customFormat="false" ht="33.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="149" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B32" s="150" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C32" s="151" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D32" s="152" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E32" s="153"/>
       <c r="F32" s="154" t="n">
@@ -6349,7 +6355,7 @@
         <v>15</v>
       </c>
       <c r="L32" s="160" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M32" s="151"/>
       <c r="N32" s="161"/>
@@ -6357,22 +6363,22 @@
       <c r="P32" s="163"/>
       <c r="Q32" s="164"/>
       <c r="R32" s="165" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="S32" s="166"/>
       <c r="T32" s="167"/>
     </row>
     <row r="33" customFormat="false" ht="22.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="135" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B33" s="168" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C33" s="169"/>
       <c r="D33" s="170"/>
       <c r="E33" s="171" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F33" s="172" t="n">
         <v>42855</v>
@@ -6385,28 +6391,28 @@
         <v>10787</v>
       </c>
       <c r="J33" s="174" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K33" s="175"/>
       <c r="L33" s="176"/>
       <c r="M33" s="177" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="N33" s="178"/>
       <c r="O33" s="179"/>
       <c r="P33" s="180" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="Q33" s="181"/>
       <c r="R33" s="182" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="S33" s="183"/>
       <c r="T33" s="184"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="185" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B34" s="86"/>
       <c r="C34" s="186"/>
@@ -6452,7 +6458,7 @@
     </row>
     <row r="36" s="192" customFormat="true" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="191" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B36" s="191"/>
       <c r="C36" s="191"/>
@@ -6476,7 +6482,7 @@
     </row>
     <row r="37" s="192" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="193" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B37" s="193"/>
       <c r="C37" s="193"/>
@@ -6500,7 +6506,7 @@
     </row>
     <row r="38" s="192" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="193" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B38" s="193"/>
       <c r="C38" s="193"/>
@@ -6524,7 +6530,7 @@
     </row>
     <row r="39" s="192" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="193" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B39" s="193"/>
       <c r="C39" s="193"/>
@@ -6548,7 +6554,7 @@
     </row>
     <row r="40" s="192" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="193" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B40" s="193"/>
       <c r="C40" s="193"/>
@@ -6572,7 +6578,7 @@
     </row>
     <row r="41" s="192" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="193" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B41" s="193"/>
       <c r="C41" s="193"/>
@@ -6698,7 +6704,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="84" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="84" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="84" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="84" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="84" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="84" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="84" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="84" width="6.71"/>
@@ -6718,7 +6724,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="85" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B1" s="86"/>
       <c r="C1" s="86"/>
@@ -6746,7 +6752,7 @@
     </row>
     <row r="2" s="200" customFormat="true" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="196" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B2" s="197"/>
       <c r="C2" s="197"/>
@@ -6778,15 +6784,15 @@
     </row>
     <row r="3" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="88" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C3" s="89"/>
       <c r="D3" s="89"/>
       <c r="E3" s="89" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F3" s="89"/>
       <c r="G3" s="89"/>
@@ -6800,34 +6806,34 @@
       <c r="O3" s="89"/>
       <c r="P3" s="89"/>
       <c r="Q3" s="90" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="R3" s="90"/>
       <c r="S3" s="90" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T3" s="90"/>
       <c r="U3" s="90" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="V3" s="90"/>
       <c r="W3" s="91" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="X3" s="91"/>
       <c r="Y3" s="201"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="202" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" s="203" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C4" s="203"/>
       <c r="D4" s="203"/>
       <c r="E4" s="204" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F4" s="204"/>
       <c r="G4" s="204"/>
@@ -6841,34 +6847,34 @@
       <c r="O4" s="204"/>
       <c r="P4" s="204"/>
       <c r="Q4" s="205" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="R4" s="205"/>
       <c r="S4" s="205" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T4" s="205"/>
       <c r="U4" s="205" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V4" s="205"/>
       <c r="W4" s="101" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X4" s="101"/>
       <c r="Y4" s="201"/>
     </row>
     <row r="5" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="97" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B5" s="98" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" s="98"/>
       <c r="D5" s="98"/>
       <c r="E5" s="99" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F5" s="99"/>
       <c r="G5" s="99"/>
@@ -6886,7 +6892,7 @@
       <c r="S5" s="100"/>
       <c r="T5" s="100"/>
       <c r="U5" s="100" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V5" s="100"/>
       <c r="W5" s="102"/>
@@ -6895,15 +6901,15 @@
     </row>
     <row r="6" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="97" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C6" s="98"/>
       <c r="D6" s="98"/>
       <c r="E6" s="99" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F6" s="99"/>
       <c r="G6" s="99"/>
@@ -6917,34 +6923,34 @@
       <c r="O6" s="99"/>
       <c r="P6" s="99"/>
       <c r="Q6" s="100" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="R6" s="100"/>
       <c r="S6" s="100" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="T6" s="100"/>
       <c r="U6" s="100" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="V6" s="100"/>
       <c r="W6" s="206" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="X6" s="206"/>
       <c r="Y6" s="201"/>
     </row>
     <row r="7" customFormat="false" ht="110.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="97" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C7" s="98"/>
       <c r="D7" s="98"/>
       <c r="E7" s="99" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F7" s="99"/>
       <c r="G7" s="99"/>
@@ -6969,15 +6975,15 @@
     </row>
     <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="97" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C8" s="98"/>
       <c r="D8" s="98"/>
       <c r="E8" s="99" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F8" s="99"/>
       <c r="G8" s="99"/>
@@ -6991,24 +6997,24 @@
       <c r="O8" s="99"/>
       <c r="P8" s="99"/>
       <c r="Q8" s="100" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="R8" s="100"/>
       <c r="S8" s="100"/>
       <c r="T8" s="100"/>
       <c r="U8" s="100" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="V8" s="100"/>
       <c r="W8" s="102" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X8" s="102"/>
       <c r="Y8" s="201"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="97" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B9" s="98" t="s">
         <v>57</v>
@@ -7016,7 +7022,7 @@
       <c r="C9" s="98"/>
       <c r="D9" s="98"/>
       <c r="E9" s="99" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="F9" s="99"/>
       <c r="G9" s="99"/>
@@ -7032,7 +7038,7 @@
       <c r="Q9" s="100"/>
       <c r="R9" s="100"/>
       <c r="S9" s="100" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="T9" s="100"/>
       <c r="U9" s="100"/>
@@ -7043,15 +7049,15 @@
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="97" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B10" s="98" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C10" s="98"/>
       <c r="D10" s="98"/>
       <c r="E10" s="99" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F10" s="99"/>
       <c r="G10" s="99"/>
@@ -7067,11 +7073,11 @@
       <c r="Q10" s="100"/>
       <c r="R10" s="100"/>
       <c r="S10" s="100" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="T10" s="100"/>
       <c r="U10" s="100" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="V10" s="100"/>
       <c r="W10" s="102"/>
@@ -7080,15 +7086,15 @@
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="97" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C11" s="98"/>
       <c r="D11" s="98"/>
       <c r="E11" s="99" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F11" s="99"/>
       <c r="G11" s="99"/>
@@ -7113,15 +7119,15 @@
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="97" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B12" s="98" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C12" s="98"/>
       <c r="D12" s="98"/>
       <c r="E12" s="99" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F12" s="99"/>
       <c r="G12" s="99"/>
@@ -7146,15 +7152,15 @@
     </row>
     <row r="13" customFormat="false" ht="68.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="97" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B13" s="103" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C13" s="103"/>
       <c r="D13" s="103"/>
       <c r="E13" s="99" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F13" s="99"/>
       <c r="G13" s="99"/>
@@ -7168,34 +7174,34 @@
       <c r="O13" s="99"/>
       <c r="P13" s="99"/>
       <c r="Q13" s="100" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="R13" s="100"/>
       <c r="S13" s="100" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="T13" s="100"/>
       <c r="U13" s="100" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="V13" s="100"/>
       <c r="W13" s="102" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="X13" s="102"/>
       <c r="Y13" s="201"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="97" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B14" s="98" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C14" s="98"/>
       <c r="D14" s="98"/>
       <c r="E14" s="99" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F14" s="99"/>
       <c r="G14" s="99"/>
@@ -7220,15 +7226,15 @@
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="97" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B15" s="98" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C15" s="98"/>
       <c r="D15" s="98"/>
       <c r="E15" s="99" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F15" s="99"/>
       <c r="G15" s="99"/>
@@ -7253,15 +7259,15 @@
     </row>
     <row r="16" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="97" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C16" s="98"/>
       <c r="D16" s="98"/>
       <c r="E16" s="99" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F16" s="99"/>
       <c r="G16" s="99"/>
@@ -7286,15 +7292,15 @@
     </row>
     <row r="17" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="97" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B17" s="98" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C17" s="98"/>
       <c r="D17" s="98"/>
       <c r="E17" s="99" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F17" s="99"/>
       <c r="G17" s="99"/>
@@ -7308,34 +7314,34 @@
       <c r="O17" s="99"/>
       <c r="P17" s="99"/>
       <c r="Q17" s="99" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="R17" s="99"/>
       <c r="S17" s="100" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="T17" s="100"/>
       <c r="U17" s="100" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="V17" s="100"/>
       <c r="W17" s="206" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="X17" s="206"/>
       <c r="Y17" s="201"/>
     </row>
     <row r="18" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="97" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B18" s="104" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C18" s="104"/>
       <c r="D18" s="104"/>
       <c r="E18" s="99" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F18" s="99"/>
       <c r="G18" s="99"/>
@@ -7360,15 +7366,15 @@
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="97" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B19" s="98" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C19" s="98"/>
       <c r="D19" s="98"/>
       <c r="E19" s="99" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F19" s="99"/>
       <c r="G19" s="99"/>
@@ -7386,7 +7392,7 @@
       <c r="S19" s="100"/>
       <c r="T19" s="100"/>
       <c r="U19" s="100" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="V19" s="100"/>
       <c r="W19" s="102"/>
@@ -7395,15 +7401,15 @@
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="97" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B20" s="98" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C20" s="98"/>
       <c r="D20" s="98"/>
       <c r="E20" s="99" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F20" s="99"/>
       <c r="G20" s="99"/>
@@ -7428,15 +7434,15 @@
     </row>
     <row r="21" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="105" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B21" s="106" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C21" s="106"/>
       <c r="D21" s="106"/>
       <c r="E21" s="99" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F21" s="99"/>
       <c r="G21" s="99"/>
@@ -7461,15 +7467,15 @@
     </row>
     <row r="22" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="107" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B22" s="108" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C22" s="108"/>
       <c r="D22" s="108"/>
       <c r="E22" s="109" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F22" s="109"/>
       <c r="G22" s="109"/>

</xml_diff>